<commit_message>
updated the code with many flags. finding balancing triplets automagically now
</commit_message>
<xml_diff>
--- a/docs/choosing_triplets_new_range2.xlsx
+++ b/docs/choosing_triplets_new_range2.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="21">
   <si>
     <t>simulation name</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>regular</t>
+  </si>
+  <si>
+    <t>practice</t>
+  </si>
+  <si>
+    <t>query_img_idx</t>
+  </si>
+  <si>
+    <t>ref1_img_idx</t>
+  </si>
+  <si>
+    <t>ref2_img_idx</t>
   </si>
 </sst>
 </file>
@@ -556,11 +568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +588,7 @@
     <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,8 +625,17 @@
       <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -659,21 +680,33 @@
       <c r="L2" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>E2-1</f>
+        <v>45</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:O2" si="0">F2-1</f>
+        <v>37</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="15">
-        <f t="shared" ref="B3:B28" si="0">E3-F3</f>
+        <f t="shared" ref="B3:B28" si="1">E3-F3</f>
         <v>8</v>
       </c>
       <c r="C3" s="15">
-        <f t="shared" ref="C3:C28" si="1">E3-G3</f>
+        <f t="shared" ref="C3:C28" si="2">E3-G3</f>
         <v>-8</v>
       </c>
       <c r="D3" s="16">
-        <f t="shared" ref="D3:D28" si="2">F3-G3</f>
+        <f t="shared" ref="D3:D28" si="3">F3-G3</f>
         <v>-16</v>
       </c>
       <c r="E3" s="5">
@@ -688,15 +721,15 @@
         <v>86</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" ref="H3:H28" si="3">ABS(B3)</f>
+        <f t="shared" ref="H3:H28" si="4">ABS(B3)</f>
         <v>8</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3:I28" si="4">ABS(C3)</f>
+        <f t="shared" ref="I3:I28" si="5">ABS(C3)</f>
         <v>8</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J28" si="5">ABS(D3)</f>
+        <f t="shared" ref="J3:J28" si="6">ABS(D3)</f>
         <v>16</v>
       </c>
       <c r="K3" s="10" t="s">
@@ -705,21 +738,33 @@
       <c r="L3" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f t="shared" ref="M3:M52" si="7">E3-1</f>
+        <v>77</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N52" si="8">F3-1</f>
+        <v>69</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O52" si="9">G3-1</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C4" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="D4" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-16</v>
       </c>
       <c r="E4" s="5">
@@ -734,15 +779,15 @@
         <v>120</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="K4" s="10" t="s">
@@ -751,21 +796,33 @@
       <c r="L4" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" si="7"/>
+        <v>111</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="8"/>
+        <v>103</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C5" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D5" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E5" s="5">
@@ -780,15 +837,15 @@
         <v>62</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I5" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K5" s="10" t="s">
@@ -797,21 +854,33 @@
       <c r="L5" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C6" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D6" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E6" s="5">
@@ -826,15 +895,15 @@
         <v>94</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K6" s="10" t="s">
@@ -843,21 +912,33 @@
       <c r="L6" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="8"/>
+        <v>61</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="9"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C7" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D7" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E7" s="5">
@@ -872,15 +953,15 @@
         <v>120</v>
       </c>
       <c r="H7" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K7" s="10" t="s">
@@ -889,21 +970,33 @@
       <c r="L7" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="19">
-        <f t="shared" ref="B8" si="6">E8-F8</f>
+        <f t="shared" ref="B8" si="10">E8-F8</f>
         <v>24</v>
       </c>
       <c r="C8" s="19">
-        <f t="shared" ref="C8" si="7">E8-G8</f>
+        <f t="shared" ref="C8" si="11">E8-G8</f>
         <v>-24</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" ref="D8" si="8">F8-G8</f>
+        <f t="shared" ref="D8" si="12">F8-G8</f>
         <v>-48</v>
       </c>
       <c r="E8" s="5">
@@ -918,15 +1011,15 @@
         <v>78</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" ref="H8" si="9">ABS(B8)</f>
+        <f t="shared" ref="H8" si="13">ABS(B8)</f>
         <v>24</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" ref="I8" si="10">ABS(C8)</f>
+        <f t="shared" ref="I8" si="14">ABS(C8)</f>
         <v>24</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" ref="J8" si="11">ABS(D8)</f>
+        <f t="shared" ref="J8" si="15">ABS(D8)</f>
         <v>48</v>
       </c>
       <c r="K8" s="10" t="s">
@@ -935,21 +1028,33 @@
       <c r="L8" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="9"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C9" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-48</v>
       </c>
       <c r="E9" s="5">
@@ -964,15 +1069,15 @@
         <v>102</v>
       </c>
       <c r="H9" s="5">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="I9" s="5">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
+      <c r="I9" s="5">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
       <c r="J9" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="K9" s="10" t="s">
@@ -981,21 +1086,33 @@
       <c r="L9" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="8"/>
+        <v>53</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="9"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C10" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-48</v>
       </c>
       <c r="E10" s="5">
@@ -1010,15 +1127,15 @@
         <v>118</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="I10" s="5">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
+      <c r="I10" s="5">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
       <c r="J10" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="K10" s="10" t="s">
@@ -1027,21 +1144,33 @@
       <c r="L10" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>93</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="9"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C11" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D11" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="E11" s="5">
@@ -1056,15 +1185,15 @@
         <v>54</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K11" s="10" t="s">
@@ -1073,21 +1202,33 @@
       <c r="L11" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C12" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D12" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="E12" s="5">
@@ -1102,15 +1243,15 @@
         <v>94</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K12" s="10" t="s">
@@ -1119,21 +1260,33 @@
       <c r="L12" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="9"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C13" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D13" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="E13" s="5">
@@ -1148,15 +1301,15 @@
         <v>120</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K13" s="10" t="s">
@@ -1165,21 +1318,33 @@
       <c r="L13" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="8"/>
+        <v>95</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C14" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="D14" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="E14" s="5">
@@ -1194,15 +1359,15 @@
         <v>54</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K14" s="10" t="s">
@@ -1211,21 +1376,33 @@
       <c r="L14" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C15" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="D15" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="E15" s="5">
@@ -1240,15 +1417,15 @@
         <v>86</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K15" s="10" t="s">
@@ -1257,21 +1434,33 @@
       <c r="L15" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="8"/>
+        <v>61</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="9"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C16" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="D16" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="E16" s="5">
@@ -1286,15 +1475,15 @@
         <v>120</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K16" s="10" t="s">
@@ -1303,21 +1492,33 @@
       <c r="L16" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>111</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="8"/>
+        <v>95</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C17" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D17" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="E17" s="5">
@@ -1332,15 +1533,15 @@
         <v>70</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="K17" s="10" t="s">
@@ -1349,21 +1550,33 @@
       <c r="L17" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="9"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C18" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D18" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="E18" s="5">
@@ -1378,15 +1591,15 @@
         <v>102</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I18" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="K18" s="10" t="s">
@@ -1395,21 +1608,33 @@
       <c r="L18" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="8"/>
+        <v>61</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="9"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C19" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D19" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="E19" s="5">
@@ -1424,15 +1649,15 @@
         <v>120</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="K19" s="10" t="s">
@@ -1441,21 +1666,33 @@
       <c r="L19" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="8"/>
+        <v>79</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C20" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D20" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="E20" s="5">
@@ -1470,15 +1707,15 @@
         <v>70</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I20" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J20" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="K20" s="10" t="s">
@@ -1487,21 +1724,33 @@
       <c r="L20" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="9"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C21" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D21" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="E21" s="5">
@@ -1516,15 +1765,15 @@
         <v>94</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J21" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="K21" s="10" t="s">
@@ -1533,21 +1782,33 @@
       <c r="L21" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="8"/>
+        <v>53</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="9"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C22" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="D22" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="E22" s="5">
@@ -1562,15 +1823,15 @@
         <v>120</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I22" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="K22" s="10" t="s">
@@ -1579,21 +1840,33 @@
       <c r="L22" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="8"/>
+        <v>79</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C23" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D23" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E23" s="5">
@@ -1608,15 +1881,15 @@
         <v>62</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I23" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K23" s="10" t="s">
@@ -1625,21 +1898,33 @@
       <c r="L23" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C24" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D24" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E24" s="5">
@@ -1654,15 +1939,15 @@
         <v>102</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I24" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K24" s="10" t="s">
@@ -1671,44 +1956,56 @@
       <c r="L24" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="9"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C25" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="D25" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E25" s="5">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F25" s="13">
         <f>E25-Sheet2!$B$1*1</f>
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G25" s="13">
         <f>E25+Sheet2!$B$1*3</f>
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I25" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K25" s="10" t="s">
@@ -1717,21 +2014,33 @@
       <c r="L25" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C26" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="D26" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E26" s="5">
@@ -1746,15 +2055,15 @@
         <v>62</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I26" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J26" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K26" s="10" t="s">
@@ -1763,21 +2072,33 @@
       <c r="L26" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <f t="shared" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C27" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="D27" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E27" s="5">
@@ -1792,15 +2113,15 @@
         <v>86</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I27" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J27" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K27" s="10" t="s">
@@ -1809,21 +2130,33 @@
       <c r="L27" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="8"/>
+        <v>53</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="9"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C28" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="D28" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="E28" s="5">
@@ -1838,15 +2171,15 @@
         <v>120</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I28" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="K28" s="10" t="s">
@@ -1855,21 +2188,33 @@
       <c r="L28" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <f t="shared" si="7"/>
+        <v>111</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="4">
-        <f t="shared" ref="B29:B30" si="12">E29-F29</f>
+        <f t="shared" ref="B29:B30" si="16">E29-F29</f>
         <v>8</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" ref="C29:C30" si="13">E29-G29</f>
+        <f t="shared" ref="C29:C30" si="17">E29-G29</f>
         <v>-78</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" ref="D29:D30" si="14">F29-G29</f>
+        <f t="shared" ref="D29:D30" si="18">F29-G29</f>
         <v>-86</v>
       </c>
       <c r="E29" s="4">
@@ -1882,15 +2227,15 @@
         <v>116</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" ref="H29:H30" si="15">ABS(B29)</f>
+        <f t="shared" ref="H29:H30" si="19">ABS(B29)</f>
         <v>8</v>
       </c>
       <c r="I29" s="5">
-        <f t="shared" ref="I29:I30" si="16">ABS(C29)</f>
+        <f t="shared" ref="I29:I30" si="20">ABS(C29)</f>
         <v>78</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" ref="J29:J30" si="17">ABS(D29)</f>
+        <f t="shared" ref="J29:J30" si="21">ABS(D29)</f>
         <v>86</v>
       </c>
       <c r="K29" s="10" t="s">
@@ -1899,21 +2244,33 @@
       <c r="L29" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="9"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="C30" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-78</v>
       </c>
       <c r="D30" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-86</v>
       </c>
       <c r="E30" s="4">
@@ -1926,15 +2283,15 @@
         <v>116</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="I30" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>78</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>86</v>
       </c>
       <c r="K30" s="10" t="s">
@@ -1943,21 +2300,33 @@
       <c r="L30" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="9"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="4">
-        <f t="shared" ref="B31:B52" si="18">E31-F31</f>
+        <f t="shared" ref="B31:B52" si="22">E31-F31</f>
         <v>8</v>
       </c>
       <c r="C31" s="4">
-        <f t="shared" ref="C31:C52" si="19">E31-G31</f>
+        <f t="shared" ref="C31:C52" si="23">E31-G31</f>
         <v>-78</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" ref="D31:D52" si="20">F31-G31</f>
+        <f t="shared" ref="D31:D52" si="24">F31-G31</f>
         <v>-86</v>
       </c>
       <c r="E31" s="4">
@@ -1970,15 +2339,15 @@
         <v>116</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" ref="H31:H52" si="21">ABS(B31)</f>
+        <f t="shared" ref="H31:H52" si="25">ABS(B31)</f>
         <v>8</v>
       </c>
       <c r="I31" s="5">
-        <f t="shared" ref="I31:I52" si="22">ABS(C31)</f>
+        <f t="shared" ref="I31:I52" si="26">ABS(C31)</f>
         <v>78</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" ref="J31:J52" si="23">ABS(D31)</f>
+        <f t="shared" ref="J31:J52" si="27">ABS(D31)</f>
         <v>86</v>
       </c>
       <c r="K31" s="10" t="s">
@@ -1987,21 +2356,33 @@
       <c r="L31" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="9"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-78</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-86</v>
       </c>
       <c r="E32" s="4">
@@ -2014,15 +2395,15 @@
         <v>116</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>8</v>
       </c>
       <c r="I32" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>78</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>86</v>
       </c>
       <c r="K32" s="10" t="s">
@@ -2031,21 +2412,33 @@
       <c r="L32" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="9"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>16</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-46</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-62</v>
       </c>
       <c r="E33" s="4">
@@ -2058,15 +2451,15 @@
         <v>108</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>16</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>46</v>
       </c>
       <c r="J33" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>62</v>
       </c>
       <c r="K33" s="10" t="s">
@@ -2075,21 +2468,33 @@
       <c r="L33" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <f t="shared" si="7"/>
+        <v>61</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="9"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>16</v>
       </c>
       <c r="C34" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-46</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-62</v>
       </c>
       <c r="E34" s="4">
@@ -2102,15 +2507,15 @@
         <v>108</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>16</v>
       </c>
       <c r="I34" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>46</v>
       </c>
       <c r="J34" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>62</v>
       </c>
       <c r="K34" s="10" t="s">
@@ -2119,21 +2524,33 @@
       <c r="L34" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <f t="shared" si="7"/>
+        <v>61</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="9"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B35" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="C35" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-24</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-32</v>
       </c>
       <c r="E35" s="4">
@@ -2146,654 +2563,834 @@
         <v>70</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>8</v>
       </c>
       <c r="I35" s="4">
+        <f t="shared" si="26"/>
+        <v>24</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="27"/>
+        <v>32</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="8"/>
+        <v>37</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="9"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="23"/>
+        <v>-24</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="24"/>
+        <v>-32</v>
+      </c>
+      <c r="E36" s="4">
+        <v>46</v>
+      </c>
+      <c r="F36" s="4">
+        <v>38</v>
+      </c>
+      <c r="G36" s="4">
+        <v>70</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" si="25"/>
+        <v>8</v>
+      </c>
+      <c r="I36" s="4">
+        <f t="shared" si="26"/>
+        <v>24</v>
+      </c>
+      <c r="J36" s="4">
+        <f t="shared" si="27"/>
+        <v>32</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="8"/>
+        <v>37</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="9"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="4">
+        <f t="shared" si="22"/>
+        <v>-12</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="24"/>
+        <v>28</v>
+      </c>
+      <c r="E37" s="4">
+        <v>108</v>
+      </c>
+      <c r="F37" s="4">
+        <v>120</v>
+      </c>
+      <c r="G37" s="4">
+        <v>92</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="25"/>
+        <v>12</v>
+      </c>
+      <c r="I37" s="4">
+        <f t="shared" si="26"/>
+        <v>16</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" si="27"/>
+        <v>28</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="7"/>
+        <v>107</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="8"/>
+        <v>119</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="9"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="4">
+        <f t="shared" si="22"/>
+        <v>-12</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="24"/>
+        <v>28</v>
+      </c>
+      <c r="E38" s="4">
+        <v>108</v>
+      </c>
+      <c r="F38" s="4">
+        <v>120</v>
+      </c>
+      <c r="G38" s="4">
+        <v>92</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="25"/>
+        <v>12</v>
+      </c>
+      <c r="I38" s="4">
+        <f t="shared" si="26"/>
+        <v>16</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="27"/>
+        <v>28</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="7"/>
+        <v>107</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="8"/>
+        <v>119</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="9"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="4">
+        <f t="shared" si="22"/>
+        <v>10</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" si="23"/>
+        <v>-8</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="24"/>
+        <v>-18</v>
+      </c>
+      <c r="E39" s="4">
+        <v>110</v>
+      </c>
+      <c r="F39" s="4">
+        <v>100</v>
+      </c>
+      <c r="G39" s="4">
+        <v>118</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="I39" s="4">
+        <f t="shared" si="26"/>
+        <v>8</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="27"/>
+        <v>18</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="7"/>
+        <v>109</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="8"/>
+        <v>99</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="9"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="4">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" si="23"/>
+        <v>-14</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="24"/>
+        <v>-30</v>
+      </c>
+      <c r="E40" s="4">
+        <v>100</v>
+      </c>
+      <c r="F40" s="4">
+        <v>84</v>
+      </c>
+      <c r="G40" s="4">
+        <v>114</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" si="25"/>
+        <v>16</v>
+      </c>
+      <c r="I40" s="4">
+        <f t="shared" si="26"/>
+        <v>14</v>
+      </c>
+      <c r="J40" s="4">
+        <f t="shared" si="27"/>
+        <v>30</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="8"/>
+        <v>83</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="9"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="4">
+        <f t="shared" si="22"/>
+        <v>10</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" si="23"/>
+        <v>-8</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="24"/>
+        <v>-18</v>
+      </c>
+      <c r="E41" s="4">
+        <v>98</v>
+      </c>
+      <c r="F41" s="4">
+        <v>88</v>
+      </c>
+      <c r="G41" s="4">
+        <v>106</v>
+      </c>
+      <c r="H41" s="4">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="I41" s="4">
+        <f t="shared" si="26"/>
+        <v>8</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" si="27"/>
+        <v>18</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="7"/>
+        <v>97</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="9"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="4">
+        <f t="shared" si="22"/>
+        <v>10</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="23"/>
+        <v>-8</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="24"/>
+        <v>-18</v>
+      </c>
+      <c r="E42" s="4">
+        <v>98</v>
+      </c>
+      <c r="F42" s="4">
+        <v>88</v>
+      </c>
+      <c r="G42" s="4">
+        <v>106</v>
+      </c>
+      <c r="H42" s="4">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="I42" s="4">
+        <f t="shared" si="26"/>
+        <v>8</v>
+      </c>
+      <c r="J42" s="4">
+        <f t="shared" si="27"/>
+        <v>18</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="7"/>
+        <v>97</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="9"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="4">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="23"/>
+        <v>-20</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="24"/>
+        <v>-36</v>
+      </c>
+      <c r="E43" s="4">
+        <v>100</v>
+      </c>
+      <c r="F43" s="4">
+        <v>84</v>
+      </c>
+      <c r="G43" s="4">
+        <v>120</v>
+      </c>
+      <c r="H43" s="4">
+        <f t="shared" si="25"/>
+        <v>16</v>
+      </c>
+      <c r="I43" s="4">
+        <f t="shared" si="26"/>
+        <v>20</v>
+      </c>
+      <c r="J43" s="4">
+        <f t="shared" si="27"/>
+        <v>36</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="8"/>
+        <v>83</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="4">
+        <f t="shared" si="22"/>
+        <v>26</v>
+      </c>
+      <c r="C44" s="4">
+        <f t="shared" si="23"/>
+        <v>-10</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" si="24"/>
+        <v>-36</v>
+      </c>
+      <c r="E44" s="4">
+        <v>110</v>
+      </c>
+      <c r="F44" s="4">
+        <v>84</v>
+      </c>
+      <c r="G44" s="4">
+        <v>120</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" si="25"/>
+        <v>26</v>
+      </c>
+      <c r="I44" s="4">
+        <f t="shared" si="26"/>
+        <v>10</v>
+      </c>
+      <c r="J44" s="4">
+        <f t="shared" si="27"/>
+        <v>36</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="7"/>
+        <v>109</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="8"/>
+        <v>83</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="4">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="C45" s="4">
+        <f t="shared" si="23"/>
+        <v>-24</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" si="24"/>
+        <v>-40</v>
+      </c>
+      <c r="E45" s="4">
+        <v>46</v>
+      </c>
+      <c r="F45" s="4">
+        <v>30</v>
+      </c>
+      <c r="G45" s="4">
+        <v>70</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" si="25"/>
+        <v>16</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" si="26"/>
+        <v>24</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" si="27"/>
+        <v>40</v>
+      </c>
+      <c r="K45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="9"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="4">
+        <f t="shared" si="22"/>
+        <v>-8</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="23"/>
+        <v>32</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="24"/>
+        <v>40</v>
+      </c>
+      <c r="E46" s="4">
+        <v>62</v>
+      </c>
+      <c r="F46" s="4">
+        <v>70</v>
+      </c>
+      <c r="G46" s="4">
+        <v>30</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" si="25"/>
+        <v>8</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" si="26"/>
+        <v>32</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="27"/>
+        <v>40</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="7"/>
+        <v>61</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="9"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="4">
+        <f t="shared" si="22"/>
+        <v>-16</v>
+      </c>
+      <c r="C47" s="4">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="24"/>
+        <v>24</v>
+      </c>
+      <c r="E47" s="4">
+        <v>46</v>
+      </c>
+      <c r="F47" s="4">
+        <v>62</v>
+      </c>
+      <c r="G47" s="4">
+        <v>38</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" si="25"/>
+        <v>16</v>
+      </c>
+      <c r="I47" s="4">
+        <f t="shared" si="26"/>
+        <v>8</v>
+      </c>
+      <c r="J47" s="4">
+        <f t="shared" si="27"/>
+        <v>24</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="8"/>
+        <v>61</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="9"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="4">
+        <f t="shared" si="22"/>
+        <v>-8</v>
+      </c>
+      <c r="C48" s="4">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="24"/>
+        <v>24</v>
+      </c>
+      <c r="E48" s="4">
+        <v>54</v>
+      </c>
+      <c r="F48" s="4">
+        <v>62</v>
+      </c>
+      <c r="G48" s="4">
+        <v>38</v>
+      </c>
+      <c r="H48" s="4">
+        <f t="shared" si="25"/>
+        <v>8</v>
+      </c>
+      <c r="I48" s="4">
+        <f t="shared" si="26"/>
+        <v>16</v>
+      </c>
+      <c r="J48" s="4">
+        <f t="shared" si="27"/>
+        <v>24</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="8"/>
+        <v>61</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="9"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="4">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="23"/>
+        <v>-44</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="24"/>
+        <v>-60</v>
+      </c>
+      <c r="E49" s="4">
+        <v>46</v>
+      </c>
+      <c r="F49" s="4">
+        <v>30</v>
+      </c>
+      <c r="G49" s="4">
+        <v>90</v>
+      </c>
+      <c r="H49" s="4">
+        <f t="shared" si="25"/>
+        <v>16</v>
+      </c>
+      <c r="I49" s="4">
+        <f t="shared" si="26"/>
+        <v>44</v>
+      </c>
+      <c r="J49" s="4">
+        <f t="shared" si="27"/>
+        <v>60</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="9"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="4">
         <f t="shared" si="22"/>
         <v>24</v>
       </c>
-      <c r="J35" s="4">
+      <c r="C50" s="4">
         <f t="shared" si="23"/>
-        <v>32</v>
-      </c>
-      <c r="K35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" s="4">
-        <f t="shared" si="18"/>
-        <v>8</v>
-      </c>
-      <c r="C36" s="4">
-        <f t="shared" si="19"/>
-        <v>-24</v>
-      </c>
-      <c r="D36" s="4">
-        <f t="shared" si="20"/>
-        <v>-32</v>
-      </c>
-      <c r="E36" s="4">
-        <v>46</v>
-      </c>
-      <c r="F36" s="4">
-        <v>38</v>
-      </c>
-      <c r="G36" s="4">
-        <v>70</v>
-      </c>
-      <c r="H36" s="4">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
-      <c r="I36" s="4">
-        <f t="shared" si="22"/>
-        <v>24</v>
-      </c>
-      <c r="J36" s="4">
-        <f t="shared" si="23"/>
-        <v>32</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="4">
-        <f t="shared" si="18"/>
-        <v>-12</v>
-      </c>
-      <c r="C37" s="4">
-        <f t="shared" si="19"/>
-        <v>16</v>
-      </c>
-      <c r="D37" s="4">
-        <f t="shared" si="20"/>
-        <v>28</v>
-      </c>
-      <c r="E37" s="4">
-        <v>108</v>
-      </c>
-      <c r="F37" s="4">
-        <v>120</v>
-      </c>
-      <c r="G37" s="4">
-        <v>92</v>
-      </c>
-      <c r="H37" s="4">
-        <f t="shared" si="21"/>
-        <v>12</v>
-      </c>
-      <c r="I37" s="4">
-        <f t="shared" si="22"/>
-        <v>16</v>
-      </c>
-      <c r="J37" s="4">
-        <f t="shared" si="23"/>
-        <v>28</v>
-      </c>
-      <c r="K37" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="4">
-        <f t="shared" si="18"/>
-        <v>-12</v>
-      </c>
-      <c r="C38" s="4">
-        <f t="shared" si="19"/>
-        <v>16</v>
-      </c>
-      <c r="D38" s="4">
-        <f t="shared" si="20"/>
-        <v>28</v>
-      </c>
-      <c r="E38" s="4">
-        <v>108</v>
-      </c>
-      <c r="F38" s="4">
-        <v>120</v>
-      </c>
-      <c r="G38" s="4">
-        <v>92</v>
-      </c>
-      <c r="H38" s="4">
-        <f t="shared" si="21"/>
-        <v>12</v>
-      </c>
-      <c r="I38" s="4">
-        <f t="shared" si="22"/>
-        <v>16</v>
-      </c>
-      <c r="J38" s="4">
-        <f t="shared" si="23"/>
-        <v>28</v>
-      </c>
-      <c r="K38" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="4">
-        <f t="shared" si="18"/>
-        <v>10</v>
-      </c>
-      <c r="C39" s="4">
-        <f t="shared" si="19"/>
-        <v>-8</v>
-      </c>
-      <c r="D39" s="4">
-        <f t="shared" si="20"/>
-        <v>-18</v>
-      </c>
-      <c r="E39" s="4">
-        <v>110</v>
-      </c>
-      <c r="F39" s="4">
-        <v>100</v>
-      </c>
-      <c r="G39" s="4">
-        <v>118</v>
-      </c>
-      <c r="H39" s="4">
-        <f t="shared" si="21"/>
-        <v>10</v>
-      </c>
-      <c r="I39" s="4">
-        <f t="shared" si="22"/>
-        <v>8</v>
-      </c>
-      <c r="J39" s="4">
-        <f t="shared" si="23"/>
-        <v>18</v>
-      </c>
-      <c r="K39" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" s="4">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
-      <c r="C40" s="4">
-        <f t="shared" si="19"/>
-        <v>-14</v>
-      </c>
-      <c r="D40" s="4">
-        <f t="shared" si="20"/>
-        <v>-30</v>
-      </c>
-      <c r="E40" s="4">
-        <v>100</v>
-      </c>
-      <c r="F40" s="4">
-        <v>84</v>
-      </c>
-      <c r="G40" s="4">
-        <v>114</v>
-      </c>
-      <c r="H40" s="4">
-        <f t="shared" si="21"/>
-        <v>16</v>
-      </c>
-      <c r="I40" s="4">
-        <f t="shared" si="22"/>
-        <v>14</v>
-      </c>
-      <c r="J40" s="4">
-        <f t="shared" si="23"/>
-        <v>30</v>
-      </c>
-      <c r="K40" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="4">
-        <f t="shared" si="18"/>
-        <v>10</v>
-      </c>
-      <c r="C41" s="4">
-        <f t="shared" si="19"/>
-        <v>-8</v>
-      </c>
-      <c r="D41" s="4">
-        <f t="shared" si="20"/>
-        <v>-18</v>
-      </c>
-      <c r="E41" s="4">
-        <v>98</v>
-      </c>
-      <c r="F41" s="4">
-        <v>88</v>
-      </c>
-      <c r="G41" s="4">
-        <v>106</v>
-      </c>
-      <c r="H41" s="4">
-        <f t="shared" si="21"/>
-        <v>10</v>
-      </c>
-      <c r="I41" s="4">
-        <f t="shared" si="22"/>
-        <v>8</v>
-      </c>
-      <c r="J41" s="4">
-        <f t="shared" si="23"/>
-        <v>18</v>
-      </c>
-      <c r="K41" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="4">
-        <f t="shared" si="18"/>
-        <v>10</v>
-      </c>
-      <c r="C42" s="4">
-        <f t="shared" si="19"/>
-        <v>-8</v>
-      </c>
-      <c r="D42" s="4">
-        <f t="shared" si="20"/>
-        <v>-18</v>
-      </c>
-      <c r="E42" s="4">
-        <v>98</v>
-      </c>
-      <c r="F42" s="4">
-        <v>88</v>
-      </c>
-      <c r="G42" s="4">
-        <v>106</v>
-      </c>
-      <c r="H42" s="4">
-        <f t="shared" si="21"/>
-        <v>10</v>
-      </c>
-      <c r="I42" s="4">
-        <f t="shared" si="22"/>
-        <v>8</v>
-      </c>
-      <c r="J42" s="4">
-        <f t="shared" si="23"/>
-        <v>18</v>
-      </c>
-      <c r="K42" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" s="4">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
-      <c r="C43" s="4">
-        <f t="shared" si="19"/>
-        <v>-20</v>
-      </c>
-      <c r="D43" s="4">
-        <f t="shared" si="20"/>
-        <v>-36</v>
-      </c>
-      <c r="E43" s="4">
-        <v>100</v>
-      </c>
-      <c r="F43" s="4">
-        <v>84</v>
-      </c>
-      <c r="G43" s="4">
-        <v>120</v>
-      </c>
-      <c r="H43" s="4">
-        <f t="shared" si="21"/>
-        <v>16</v>
-      </c>
-      <c r="I43" s="4">
-        <f t="shared" si="22"/>
-        <v>20</v>
-      </c>
-      <c r="J43" s="4">
-        <f t="shared" si="23"/>
-        <v>36</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" s="4">
-        <f t="shared" si="18"/>
-        <v>26</v>
-      </c>
-      <c r="C44" s="4">
-        <f t="shared" si="19"/>
-        <v>-10</v>
-      </c>
-      <c r="D44" s="4">
-        <f t="shared" si="20"/>
-        <v>-36</v>
-      </c>
-      <c r="E44" s="4">
-        <v>110</v>
-      </c>
-      <c r="F44" s="4">
-        <v>84</v>
-      </c>
-      <c r="G44" s="4">
-        <v>120</v>
-      </c>
-      <c r="H44" s="4">
-        <f t="shared" si="21"/>
-        <v>26</v>
-      </c>
-      <c r="I44" s="4">
-        <f t="shared" si="22"/>
-        <v>10</v>
-      </c>
-      <c r="J44" s="4">
-        <f t="shared" si="23"/>
-        <v>36</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="4">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
-      <c r="C45" s="4">
-        <f t="shared" si="19"/>
-        <v>-24</v>
-      </c>
-      <c r="D45" s="4">
-        <f t="shared" si="20"/>
-        <v>-40</v>
-      </c>
-      <c r="E45" s="4">
-        <v>46</v>
-      </c>
-      <c r="F45" s="4">
-        <v>30</v>
-      </c>
-      <c r="G45" s="4">
-        <v>70</v>
-      </c>
-      <c r="H45" s="4">
-        <f t="shared" si="21"/>
-        <v>16</v>
-      </c>
-      <c r="I45" s="4">
-        <f t="shared" si="22"/>
-        <v>24</v>
-      </c>
-      <c r="J45" s="4">
-        <f t="shared" si="23"/>
-        <v>40</v>
-      </c>
-      <c r="K45" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" s="4">
-        <f t="shared" si="18"/>
-        <v>-8</v>
-      </c>
-      <c r="C46" s="4">
-        <f t="shared" si="19"/>
-        <v>32</v>
-      </c>
-      <c r="D46" s="4">
-        <f t="shared" si="20"/>
-        <v>40</v>
-      </c>
-      <c r="E46" s="4">
-        <v>62</v>
-      </c>
-      <c r="F46" s="4">
-        <v>70</v>
-      </c>
-      <c r="G46" s="4">
-        <v>30</v>
-      </c>
-      <c r="H46" s="4">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
-      <c r="I46" s="4">
-        <f t="shared" si="22"/>
-        <v>32</v>
-      </c>
-      <c r="J46" s="4">
-        <f t="shared" si="23"/>
-        <v>40</v>
-      </c>
-      <c r="K46" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="4">
-        <f t="shared" si="18"/>
-        <v>-16</v>
-      </c>
-      <c r="C47" s="4">
-        <f t="shared" si="19"/>
-        <v>8</v>
-      </c>
-      <c r="D47" s="4">
-        <f t="shared" si="20"/>
-        <v>24</v>
-      </c>
-      <c r="E47" s="4">
-        <v>46</v>
-      </c>
-      <c r="F47" s="4">
-        <v>62</v>
-      </c>
-      <c r="G47" s="4">
-        <v>38</v>
-      </c>
-      <c r="H47" s="4">
-        <f t="shared" si="21"/>
-        <v>16</v>
-      </c>
-      <c r="I47" s="4">
-        <f t="shared" si="22"/>
-        <v>8</v>
-      </c>
-      <c r="J47" s="4">
-        <f t="shared" si="23"/>
-        <v>24</v>
-      </c>
-      <c r="K47" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48" s="4">
-        <f t="shared" si="18"/>
-        <v>-8</v>
-      </c>
-      <c r="C48" s="4">
-        <f t="shared" si="19"/>
-        <v>16</v>
-      </c>
-      <c r="D48" s="4">
-        <f t="shared" si="20"/>
-        <v>24</v>
-      </c>
-      <c r="E48" s="4">
-        <v>54</v>
-      </c>
-      <c r="F48" s="4">
-        <v>62</v>
-      </c>
-      <c r="G48" s="4">
-        <v>38</v>
-      </c>
-      <c r="H48" s="4">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
-      <c r="I48" s="4">
-        <f t="shared" si="22"/>
-        <v>16</v>
-      </c>
-      <c r="J48" s="4">
-        <f t="shared" si="23"/>
-        <v>24</v>
-      </c>
-      <c r="K48" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L48" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" s="4">
-        <f t="shared" si="18"/>
-        <v>16</v>
-      </c>
-      <c r="C49" s="4">
-        <f t="shared" si="19"/>
-        <v>-44</v>
-      </c>
-      <c r="D49" s="4">
-        <f t="shared" si="20"/>
-        <v>-60</v>
-      </c>
-      <c r="E49" s="4">
-        <v>46</v>
-      </c>
-      <c r="F49" s="4">
-        <v>30</v>
-      </c>
-      <c r="G49" s="4">
-        <v>90</v>
-      </c>
-      <c r="H49" s="4">
-        <f t="shared" si="21"/>
-        <v>16</v>
-      </c>
-      <c r="I49" s="4">
-        <f t="shared" si="22"/>
-        <v>44</v>
-      </c>
-      <c r="J49" s="4">
-        <f t="shared" si="23"/>
-        <v>60</v>
-      </c>
-      <c r="K49" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="4">
-        <f t="shared" si="18"/>
-        <v>24</v>
-      </c>
-      <c r="C50" s="4">
-        <f t="shared" si="19"/>
         <v>-66</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-90</v>
       </c>
       <c r="E50" s="4">
@@ -2806,38 +3403,50 @@
         <v>120</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>24</v>
       </c>
       <c r="I50" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>66</v>
       </c>
       <c r="J50" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>90</v>
       </c>
       <c r="K50" s="10" t="s">
         <v>10</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="9"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B51" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>-8</v>
       </c>
       <c r="C51" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>20</v>
       </c>
       <c r="D51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>28</v>
       </c>
       <c r="E51" s="4">
@@ -2850,38 +3459,50 @@
         <v>92</v>
       </c>
       <c r="H51" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>8</v>
       </c>
       <c r="I51" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="J51" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>28</v>
       </c>
       <c r="K51" s="10" t="s">
         <v>10</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="7"/>
+        <v>111</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="8"/>
+        <v>119</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="9"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B52" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>40</v>
       </c>
       <c r="C52" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-14</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-54</v>
       </c>
       <c r="E52" s="4">
@@ -2894,25 +3515,37 @@
         <v>84</v>
       </c>
       <c r="H52" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>40</v>
       </c>
       <c r="I52" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>14</v>
       </c>
       <c r="J52" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>54</v>
       </c>
       <c r="K52" s="10" t="s">
         <v>10</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="9"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2926,7 +3559,7 @@
       <c r="K53" s="8"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2940,7 +3573,7 @@
       <c r="K54" s="8"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2954,7 +3587,7 @@
       <c r="K55" s="8"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2968,7 +3601,7 @@
       <c r="K56" s="8"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2982,7 +3615,7 @@
       <c r="K57" s="8"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2996,7 +3629,7 @@
       <c r="K58" s="8"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3010,7 +3643,7 @@
       <c r="K59" s="8"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3024,7 +3657,7 @@
       <c r="K60" s="8"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3038,7 +3671,7 @@
       <c r="K61" s="8"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -3052,7 +3685,7 @@
       <c r="K62" s="8"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -3066,7 +3699,7 @@
       <c r="K63" s="8"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3080,7 +3713,7 @@
       <c r="K64" s="8"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -3094,7 +3727,7 @@
       <c r="K65" s="8"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -3108,7 +3741,7 @@
       <c r="K66" s="8"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3122,7 +3755,7 @@
       <c r="K67" s="8"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3136,7 +3769,7 @@
       <c r="K68" s="8"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3150,7 +3783,7 @@
       <c r="K69" s="8"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3164,7 +3797,7 @@
       <c r="K70" s="8"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -3178,7 +3811,7 @@
       <c r="K71" s="8"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -3192,7 +3825,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -3206,7 +3839,7 @@
       <c r="K73" s="8"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -3220,7 +3853,7 @@
       <c r="K74" s="8"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -3234,7 +3867,7 @@
       <c r="K75" s="8"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -3248,7 +3881,7 @@
       <c r="K76" s="8"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -3262,7 +3895,7 @@
       <c r="K77" s="8"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -3276,7 +3909,7 @@
       <c r="K78" s="8"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -3290,7 +3923,7 @@
       <c r="K79" s="8"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -3302,8 +3935,11 @@
       <c r="I80" s="10"/>
       <c r="J80" s="10"/>
       <c r="L80" s="10"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M80"/>
+      <c r="N80"/>
+      <c r="O80"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -3316,8 +3952,11 @@
       <c r="J81" s="10"/>
       <c r="K81"/>
       <c r="L81" s="10"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M81"/>
+      <c r="N81"/>
+      <c r="O81"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -3330,8 +3969,11 @@
       <c r="J82" s="10"/>
       <c r="K82"/>
       <c r="L82" s="10"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M82"/>
+      <c r="N82"/>
+      <c r="O82"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -3344,8 +3986,11 @@
       <c r="J83" s="10"/>
       <c r="K83"/>
       <c r="L83" s="10"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M83"/>
+      <c r="N83"/>
+      <c r="O83"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -3358,8 +4003,11 @@
       <c r="J84" s="10"/>
       <c r="K84"/>
       <c r="L84" s="10"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M84"/>
+      <c r="N84"/>
+      <c r="O84"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -3372,8 +4020,11 @@
       <c r="J85" s="10"/>
       <c r="K85"/>
       <c r="L85" s="10"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M85"/>
+      <c r="N85"/>
+      <c r="O85"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -3386,8 +4037,11 @@
       <c r="J86" s="10"/>
       <c r="K86"/>
       <c r="L86" s="10"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M86"/>
+      <c r="N86"/>
+      <c r="O86"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -3400,8 +4054,11 @@
       <c r="J87" s="10"/>
       <c r="K87"/>
       <c r="L87" s="10"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M87"/>
+      <c r="N87"/>
+      <c r="O87"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -3414,8 +4071,11 @@
       <c r="J88" s="10"/>
       <c r="K88"/>
       <c r="L88" s="10"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M88"/>
+      <c r="N88"/>
+      <c r="O88"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -3427,8 +4087,11 @@
       <c r="I89" s="10"/>
       <c r="J89" s="10"/>
       <c r="L89" s="10"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89"/>
+      <c r="N89"/>
+      <c r="O89"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -3440,8 +4103,11 @@
       <c r="I90" s="10"/>
       <c r="J90" s="10"/>
       <c r="L90" s="10"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M90"/>
+      <c r="N90"/>
+      <c r="O90"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -3453,8 +4119,11 @@
       <c r="I91" s="10"/>
       <c r="J91" s="10"/>
       <c r="L91" s="10"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M91"/>
+      <c r="N91"/>
+      <c r="O91"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -3466,8 +4135,11 @@
       <c r="I92" s="10"/>
       <c r="J92" s="10"/>
       <c r="L92" s="10"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M92"/>
+      <c r="N92"/>
+      <c r="O92"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -3479,8 +4151,11 @@
       <c r="I93" s="10"/>
       <c r="J93" s="10"/>
       <c r="L93" s="10"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -3492,6 +4167,9 @@
       <c r="I94" s="10"/>
       <c r="J94" s="10"/>
       <c r="L94" s="10"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L94"/>

</xml_diff>